<commit_message>
fixed excel lock error on Windows os
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -68,6 +68,7 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -142,7 +143,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -276,7 +277,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H15" activeCellId="0" sqref="H15"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -295,10 +296,10 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="n">
-        <v>45662</v>
+        <v>45748</v>
       </c>
       <c r="B2" s="4" t="n">
-        <v>45675</v>
+        <v>45777</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>

</xml_diff>